<commit_message>
feat: added student update
</commit_message>
<xml_diff>
--- a/server/StaffsAndStudents.xlsx
+++ b/server/StaffsAndStudents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garkg\Desktop\my_projects\capstone-jeff\qit-portal-v5\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EA60AB-209B-4E28-ABFE-19C361CFD580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEDA3D0-CE85-4D3F-9678-149C96A3ED44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4A1182F0-3B78-4C16-AE2A-9B263A422355}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A1182F0-3B78-4C16-AE2A-9B263A422355}"/>
   </bookViews>
   <sheets>
     <sheet name="Staffs" sheetId="2" r:id="rId1"/>
@@ -79,33 +79,6 @@
     <t>MBA</t>
   </si>
   <si>
-    <t>2022-02-1980</t>
-  </si>
-  <si>
-    <t>2022-03-1981</t>
-  </si>
-  <si>
-    <t>2022-02-1982</t>
-  </si>
-  <si>
-    <t>2022-02-1983</t>
-  </si>
-  <si>
-    <t>2022-02-1984</t>
-  </si>
-  <si>
-    <t>2022-02-1985</t>
-  </si>
-  <si>
-    <t>2022-02-1986</t>
-  </si>
-  <si>
-    <t>2022-02-1987</t>
-  </si>
-  <si>
-    <t>2022-02-1988</t>
-  </si>
-  <si>
     <t>registrar1</t>
   </si>
   <si>
@@ -281,6 +254,33 @@
   </si>
   <si>
     <t>BSIT</t>
+  </si>
+  <si>
+    <t>2022-02-01</t>
+  </si>
+  <si>
+    <t>2022-02-02</t>
+  </si>
+  <si>
+    <t>2022-02-03</t>
+  </si>
+  <si>
+    <t>2022-02-04</t>
+  </si>
+  <si>
+    <t>2022-02-05</t>
+  </si>
+  <si>
+    <t>2022-02-06</t>
+  </si>
+  <si>
+    <t>2022-02-07</t>
+  </si>
+  <si>
+    <t>2022-02-08</t>
+  </si>
+  <si>
+    <t>2022-02-09</t>
   </si>
 </sst>
 </file>
@@ -322,8 +322,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D291706-C77A-40A1-9C53-3ABCD5639840}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,7 +651,7 @@
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="11.109375" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" customWidth="1"/>
@@ -672,7 +673,7 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
@@ -701,17 +702,17 @@
       <c r="E2">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -722,25 +723,25 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -748,25 +749,25 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>40</v>
       </c>
-      <c r="F4" t="s">
-        <v>16</v>
+      <c r="F4" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>3</v>
@@ -774,25 +775,25 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E5">
         <v>39</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
+      <c r="F5" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <v>3</v>
@@ -803,25 +804,25 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E6">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J6">
         <v>3</v>
@@ -832,25 +833,25 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E7">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -858,25 +859,25 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E8">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
-        <v>20</v>
+      <c r="F8" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -887,25 +888,25 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>35</v>
       </c>
-      <c r="F9" t="s">
-        <v>21</v>
+      <c r="F9" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -916,25 +917,25 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E10">
         <v>34</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>22</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -952,11 +953,12 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="10.5546875" style="1" customWidth="1"/>
     <col min="7" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="11" width="11.6640625" customWidth="1"/>
   </cols>
@@ -969,12 +971,12 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -984,48 +986,48 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -1033,34 +1035,34 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
+      <c r="E3" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1068,34 +1070,34 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1103,34 +1105,34 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D5">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -1138,34 +1140,34 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
+      <c r="E6" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -1173,34 +1175,34 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
+      <c r="E7" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -1216,13 +1218,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84261976-EFA2-41F0-BD82-3F5926997664}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="11.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1233,12 +1236,12 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1248,30 +1251,30 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D2">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
-        <v>14</v>
+      <c r="E2" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1279,25 +1282,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D3">
         <v>41</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
+      <c r="E3" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -1305,25 +1308,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D4">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1331,25 +1334,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
+      <c r="E5" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1357,25 +1360,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D6">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
+      <c r="E6" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1383,31 +1386,32 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D7">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>18</v>
+      <c r="E7" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>